<commit_message>
GH-130: replace ZeroCell with custom implementation
- Migrated to custom excel processor via the same apache poi lib under the hood, but w/o ZeroCell to avoid maintenance effort and improve implementation
- Added default set of type converters with auto-conversion feature
- Removed column index dependency
- Extended code coverage
- Updated readme and changelog
- Added optional debugging feature for contributors
</commit_message>
<xml_diff>
--- a/src/test/resources/random.xlsx
+++ b/src/test/resources/random.xlsx
@@ -5,104 +5,138 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+  <si>
+    <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
+  </si>
+  <si>
+    <t>Numbers Sheet Name</t>
+  </si>
+  <si>
+    <t>Numbers Table Name</t>
+  </si>
+  <si>
+    <t>Excel Worksheet Name</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
   <si>
     <t>TC</t>
   </si>
   <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>isFTE</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>phonenumber</t>
-  </si>
-  <si>
-    <t>list</t>
-  </si>
-  <si>
-    <t>testcase1</t>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Next Check</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Should Run</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Tech Stack</t>
+  </si>
+  <si>
+    <t>test1</t>
   </si>
   <si>
     <t>chrome</t>
   </si>
   <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>9876543210</t>
   </si>
   <si>
     <t>selenium,appium,restassured</t>
   </si>
   <si>
+    <t>test2</t>
+  </si>
+  <si>
     <t>edge</t>
   </si>
   <si>
-    <t>dfgdg</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>+919876543210</t>
   </si>
   <si>
     <t>docker,k8s,openshift</t>
   </si>
   <si>
-    <t>testcase2</t>
-  </si>
-  <si>
-    <t>efgh</t>
-  </si>
-  <si>
-    <t>21</t>
+    <t>test3</t>
   </si>
   <si>
     <t>postman,soapui</t>
   </si>
   <si>
-    <t>testcase3</t>
-  </si>
-  <si>
-    <t>ijkl</t>
-  </si>
-  <si>
-    <t>22</t>
+    <t>test4</t>
   </si>
   <si>
     <t>automation,performance,security</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>chromium</t>
+  </si>
+  <si>
+    <t>8291239893</t>
+  </si>
+  <si>
+    <t>allure,testng,java,gradle</t>
+  </si>
+  <si>
+    <t>Sheet2</t>
+  </si>
+  <si>
+    <t>Sheet3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="60" formatCode="yyyy-mm-dd h:mm:ss AM/PM"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -112,12 +146,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,8 +170,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -141,16 +193,106 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
@@ -160,23 +302,83 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -199,8 +401,13 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa7a7a7"/>
+      <rgbColor rgb="ff525252"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1292,225 +1499,282 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="4" width="30.5547" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" ht="0.05" customHeight="1">
+      <c r="B3" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+    </row>
+    <row r="7">
+      <c r="B7" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4"/>
+      <c r="C14" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D10" location="'Sheet1'!R1C1" tooltip="" display="Sheet1"/>
+    <hyperlink ref="D12" location="'Sheet2'!R1C1" tooltip="" display="Sheet2"/>
+    <hyperlink ref="D14" location="'Sheet3'!R1C1" tooltip="" display="Sheet3"/>
+  </hyperlinks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="9.5" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.85156" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85156" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.5" style="6" customWidth="1"/>
+    <col min="3" max="6" width="8.85156" style="6" customWidth="1"/>
+    <col min="7" max="7" width="5.85156" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.3516" style="6" customWidth="1"/>
+    <col min="9" max="9" width="28.5" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="C2" s="8">
+        <v>44700</v>
+      </c>
+      <c r="D2" s="9">
+        <v>44723.432326388887</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="F2" t="b" s="11">
+        <v>1</v>
+      </c>
+      <c r="G2" s="12">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s" s="7">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="C3" s="8">
+        <v>44660</v>
+      </c>
+      <c r="D3" s="9">
+        <v>44702.459872685184</v>
+      </c>
+      <c r="E3" s="10">
+        <v>3.546</v>
+      </c>
+      <c r="F3" t="b" s="11">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="G3" s="12">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="C4" s="8">
+        <v>44420</v>
+      </c>
+      <c r="D4" s="9">
+        <v>44958</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b" s="11">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="D2" t="b" s="3">
+      <c r="G4" s="12">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s" s="7">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" t="s" s="13">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s" s="13">
+        <v>16</v>
+      </c>
+      <c r="C5" s="14">
+        <v>44927</v>
+      </c>
+      <c r="D5" s="9">
+        <v>44906.480925925927</v>
+      </c>
+      <c r="E5" s="15">
+        <v>-1.24</v>
+      </c>
+      <c r="F5" t="b" s="16">
         <v>1</v>
       </c>
-      <c r="E2" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="D3" t="b" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s" s="2">
+      <c r="G5" s="17">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s" s="13">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="D4" t="b" s="3">
+      <c r="I5" t="s" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" t="s" s="18">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s" s="19">
+        <v>28</v>
+      </c>
+      <c r="C6" s="20">
+        <v>44620</v>
+      </c>
+      <c r="D6" s="9">
+        <v>44655.515659722223</v>
+      </c>
+      <c r="E6" s="21">
+        <v>1000</v>
+      </c>
+      <c r="F6" t="b" s="22">
         <v>1</v>
       </c>
-      <c r="E4" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="D5" t="b" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s" s="2">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="5" width="8.85156" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="4" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="G6" s="22">
+        <v>101</v>
+      </c>
+      <c r="H6" t="s" s="19">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s" s="23">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1529,79 +1793,170 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="8.85156" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="5" width="8.85156" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="8.85156" style="26" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>